<commit_message>
fix bugs - gsoc orgs
</commit_message>
<xml_diff>
--- a/GSoC-organisations-data/results.xlsx
+++ b/GSoC-organisations-data/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="605">
   <si>
     <t>ORGANISATION NAME</t>
   </si>
@@ -298,6 +298,18 @@
     <t>computational geometry,geometry processing,mesh processing,arrangement,point set processing,</t>
   </si>
   <si>
+    <t>CHAOSS</t>
+  </si>
+  <si>
+    <t>python,javascript,jupyter,mysql,elasicsearch,</t>
+  </si>
+  <si>
+    <t>Social / Communications</t>
+  </si>
+  <si>
+    <t>community,health,sustainability,metrics,</t>
+  </si>
+  <si>
     <t>Chapel</t>
   </si>
   <si>
@@ -358,15 +370,6 @@
     <t>cloud,containers,</t>
   </si>
   <si>
-    <t>CloudCV</t>
-  </si>
-  <si>
-    <t>python 3,django,aws,angularjs,docker,</t>
-  </si>
-  <si>
-    <t>machine learning,artificial intelligence,deep-learning,computer vision,</t>
-  </si>
-  <si>
     <t>coala</t>
   </si>
   <si>
@@ -406,24 +409,6 @@
     <t>copyleft,legal,nonprofit,web,creative commons,</t>
   </si>
   <si>
-    <t>CRIU (Checkpoint/Restore in User-space)</t>
-  </si>
-  <si>
-    <t>docker,linux,containers,kernel,</t>
-  </si>
-  <si>
-    <t>cloud,save/restore,load-balancing,zero-downtime,migration,</t>
-  </si>
-  <si>
-    <t>Cuneiform Digital Library Initiative (CDLI)</t>
-  </si>
-  <si>
-    <t>python,php,mysql,java,html/css,</t>
-  </si>
-  <si>
-    <t>computer vision,nlp,lod,data processing pipeline,data-collection,</t>
-  </si>
-  <si>
     <t>D Programming Language</t>
   </si>
   <si>
@@ -460,15 +445,6 @@
     <t>open government,public code,open source,web applications,open data,</t>
   </si>
   <si>
-    <t>Digital Impact Alliance</t>
-  </si>
-  <si>
-    <t>android,java,php,python,javascript,</t>
-  </si>
-  <si>
-    <t>end user application,humanitarian,international,social good,charity,</t>
-  </si>
-  <si>
     <t>Django Software Foundation</t>
   </si>
   <si>
@@ -541,15 +517,6 @@
     <t>compliance,license-scan,oss licensing,spdx,oss compliance,</t>
   </si>
   <si>
-    <t>FrameNet Brasil at the Federal University of Juiz de Fora</t>
-  </si>
-  <si>
-    <t>php,mysql,javascript,python,</t>
-  </si>
-  <si>
-    <t>natural language processing,multimodality,natural language understanding,image processing,machine translation,</t>
-  </si>
-  <si>
     <t>Free and Open Source Silicon Foundation</t>
   </si>
   <si>
@@ -583,9 +550,6 @@
     <t>c,python,ruby,openwrt,html/css/js,</t>
   </si>
   <si>
-    <t>Social / Communications</t>
-  </si>
-  <si>
     <t>network,embedded systems,web apps,wireless communications,software defined networking,</t>
   </si>
   <si>
@@ -598,15 +562,6 @@
     <t>genomics,data analysis,databases,scientific visualization,</t>
   </si>
   <si>
-    <t>GENIVI Alliance</t>
-  </si>
-  <si>
-    <t>yocto,embedded,automotive,some/ip,</t>
-  </si>
-  <si>
-    <t>automotive,graphics,communication,bigdata,embedded systems,</t>
-  </si>
-  <si>
     <t>Gentoo Foundation</t>
   </si>
   <si>
@@ -625,15 +580,6 @@
     <t>version-control,dvcs,</t>
   </si>
   <si>
-    <t>Global Alliance for Genomics and Health</t>
-  </si>
-  <si>
-    <t>java,mongodb,spring,</t>
-  </si>
-  <si>
-    <t>genomics,genetics,bioinformatics,web,standards,</t>
-  </si>
-  <si>
     <t>GNOME</t>
   </si>
   <si>
@@ -652,15 +598,6 @@
     <t>gnss,geolocation,navigation,software defined radio,communications,</t>
   </si>
   <si>
-    <t>GNU Compiler Collection</t>
-  </si>
-  <si>
-    <t>c/c++,gnu autotools,</t>
-  </si>
-  <si>
-    <t>compilers,toolchain,openmp,</t>
-  </si>
-  <si>
     <t>GNU Mailman</t>
   </si>
   <si>
@@ -677,15 +614,6 @@
   </si>
   <si>
     <t>mathematics,numerical computation,numerical methods,matlab,scientific computing,</t>
-  </si>
-  <si>
-    <t>GNU Radio</t>
-  </si>
-  <si>
-    <t>python,c++,qt,android,</t>
-  </si>
-  <si>
-    <t>software defined radio,software radio,radar,wireless communications,digital signal processing,</t>
   </si>
   <si>
     <t>Godot Engine</t>
@@ -2659,100 +2587,100 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>96</v>
       </c>
       <c r="D30" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C32" t="s">
         <v>17</v>
       </c>
       <c r="D32" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B33" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C33" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D33" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B34" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C34" t="s">
         <v>77</v>
       </c>
       <c r="D34" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B35" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C35" t="s">
         <v>77</v>
       </c>
       <c r="D35" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B36" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C36" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D36" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2763,2390 +2691,2390 @@
         <v>115</v>
       </c>
       <c r="C37" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D37" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B38" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C38" t="s">
         <v>17</v>
       </c>
       <c r="D38" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B39" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B40" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C40" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D40" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B41" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C41" t="s">
         <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
+        <v>128</v>
+      </c>
+      <c r="B42" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" t="s">
         <v>130</v>
-      </c>
-      <c r="B42" t="s">
-        <v>131</v>
-      </c>
-      <c r="C42" t="s">
-        <v>125</v>
-      </c>
-      <c r="D42" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B43" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C43" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="D43" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B44" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C44" t="s">
         <v>17</v>
       </c>
       <c r="D44" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B45" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C45" t="s">
         <v>77</v>
       </c>
       <c r="D45" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B46" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C46" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D46" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B47" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C47" t="s">
         <v>10</v>
       </c>
       <c r="D47" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B48" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C48" t="s">
         <v>10</v>
       </c>
       <c r="D48" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B49" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C49" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D49" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B50" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C50" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D50" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B51" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C51" t="s">
         <v>6</v>
       </c>
       <c r="D51" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B52" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C52" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D52" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B53" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C53" t="s">
         <v>34</v>
       </c>
       <c r="D53" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B54" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C54" t="s">
         <v>17</v>
       </c>
       <c r="D54" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B55" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C55" t="s">
         <v>10</v>
       </c>
       <c r="D55" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B56" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C56" t="s">
         <v>10</v>
       </c>
       <c r="D56" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="B57" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="C57" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="D57" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="B58" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C58" t="s">
         <v>10</v>
       </c>
       <c r="D58" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="B59" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="C59" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D59" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B60" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C60" t="s">
         <v>34</v>
       </c>
       <c r="D60" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="B61" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="C61" t="s">
-        <v>189</v>
+        <v>96</v>
       </c>
       <c r="D61" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="B62" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="C62" t="s">
         <v>6</v>
       </c>
       <c r="D62" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="B63" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="C63" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D63" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="B64" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="C64" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D64" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="B65" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="C65" t="s">
         <v>17</v>
       </c>
       <c r="D65" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="B66" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="C66" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D66" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="B67" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="C67" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D67" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="B68" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="C68" t="s">
         <v>6</v>
       </c>
       <c r="D68" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="B69" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="C69" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D69" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
       <c r="B70" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="C70" t="s">
         <v>21</v>
       </c>
       <c r="D70" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="B71" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="C71" t="s">
         <v>17</v>
       </c>
       <c r="D71" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="B72" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="C72" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D72" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="B73" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="C73" t="s">
         <v>34</v>
       </c>
       <c r="D73" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="B74" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="C74" t="s">
         <v>6</v>
       </c>
       <c r="D74" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="B75" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="C75" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D75" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="B76" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
       <c r="C76" t="s">
         <v>17</v>
       </c>
       <c r="D76" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
       <c r="B77" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="C77" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D77" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>239</v>
+        <v>215</v>
       </c>
       <c r="B78" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
       </c>
       <c r="D78" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
       <c r="B79" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="C79" t="s">
         <v>34</v>
       </c>
       <c r="D79" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
       <c r="B80" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="C80" t="s">
         <v>34</v>
       </c>
       <c r="D80" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="B81" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="C81" t="s">
         <v>34</v>
       </c>
       <c r="D81" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="B82" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="C82" t="s">
         <v>6</v>
       </c>
       <c r="D82" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
       <c r="B83" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="C83" t="s">
         <v>10</v>
       </c>
       <c r="D83" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="B84" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
       <c r="C84" t="s">
         <v>10</v>
       </c>
       <c r="D84" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
       <c r="B85" t="s">
-        <v>261</v>
+        <v>237</v>
       </c>
       <c r="C85" t="s">
         <v>21</v>
       </c>
       <c r="D85" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="B86" t="s">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="C86" t="s">
         <v>17</v>
       </c>
       <c r="D86" t="s">
-        <v>265</v>
+        <v>241</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>266</v>
+        <v>242</v>
       </c>
       <c r="B87" t="s">
-        <v>267</v>
+        <v>243</v>
       </c>
       <c r="C87" t="s">
         <v>10</v>
       </c>
       <c r="D87" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
       <c r="B88" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="C88" t="s">
         <v>17</v>
       </c>
       <c r="D88" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>272</v>
+        <v>248</v>
       </c>
       <c r="B89" t="s">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="C89" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D89" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>275</v>
+        <v>251</v>
       </c>
       <c r="B90" t="s">
-        <v>276</v>
+        <v>252</v>
       </c>
       <c r="C90" t="s">
         <v>6</v>
       </c>
       <c r="D90" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>278</v>
+        <v>254</v>
       </c>
       <c r="B91" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="C91" t="s">
         <v>17</v>
       </c>
       <c r="D91" t="s">
-        <v>280</v>
+        <v>256</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>281</v>
+        <v>257</v>
       </c>
       <c r="B92" t="s">
-        <v>282</v>
+        <v>258</v>
       </c>
       <c r="C92" t="s">
         <v>21</v>
       </c>
       <c r="D92" t="s">
-        <v>283</v>
+        <v>259</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="B93" t="s">
-        <v>285</v>
+        <v>261</v>
       </c>
       <c r="C93" t="s">
         <v>21</v>
       </c>
       <c r="D93" t="s">
-        <v>286</v>
+        <v>262</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>287</v>
+        <v>263</v>
       </c>
       <c r="B94" t="s">
-        <v>288</v>
+        <v>264</v>
       </c>
       <c r="C94" t="s">
         <v>77</v>
       </c>
       <c r="D94" t="s">
-        <v>289</v>
+        <v>265</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>290</v>
+        <v>266</v>
       </c>
       <c r="B95" t="s">
-        <v>291</v>
+        <v>267</v>
       </c>
       <c r="C95" t="s">
         <v>21</v>
       </c>
       <c r="D95" t="s">
-        <v>292</v>
+        <v>268</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>293</v>
+        <v>269</v>
       </c>
       <c r="B96" t="s">
-        <v>294</v>
+        <v>270</v>
       </c>
       <c r="C96" t="s">
         <v>17</v>
       </c>
       <c r="D96" t="s">
-        <v>295</v>
+        <v>271</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>296</v>
+        <v>272</v>
       </c>
       <c r="B97" t="s">
-        <v>297</v>
+        <v>273</v>
       </c>
       <c r="C97" t="s">
         <v>6</v>
       </c>
       <c r="D97" t="s">
-        <v>298</v>
+        <v>274</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
       <c r="B98" t="s">
-        <v>300</v>
+        <v>276</v>
       </c>
       <c r="C98" t="s">
         <v>6</v>
       </c>
       <c r="D98" t="s">
-        <v>301</v>
+        <v>277</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>302</v>
+        <v>278</v>
       </c>
       <c r="B99" t="s">
-        <v>303</v>
+        <v>279</v>
       </c>
       <c r="C99" t="s">
         <v>21</v>
       </c>
       <c r="D99" t="s">
-        <v>304</v>
+        <v>280</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>305</v>
+        <v>281</v>
       </c>
       <c r="B100" t="s">
-        <v>306</v>
+        <v>282</v>
       </c>
       <c r="C100" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D100" t="s">
-        <v>307</v>
+        <v>283</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>308</v>
+        <v>284</v>
       </c>
       <c r="B101" t="s">
-        <v>309</v>
+        <v>285</v>
       </c>
       <c r="C101" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D101" t="s">
-        <v>310</v>
+        <v>286</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>311</v>
+        <v>287</v>
       </c>
       <c r="B102" t="s">
-        <v>312</v>
+        <v>288</v>
       </c>
       <c r="C102" t="s">
         <v>10</v>
       </c>
       <c r="D102" t="s">
-        <v>313</v>
+        <v>289</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>314</v>
+        <v>290</v>
       </c>
       <c r="B103" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="C103" t="s">
         <v>17</v>
       </c>
       <c r="D103" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>317</v>
+        <v>293</v>
       </c>
       <c r="B104" t="s">
-        <v>318</v>
+        <v>294</v>
       </c>
       <c r="C104" t="s">
         <v>17</v>
       </c>
       <c r="D104" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="B105" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
       <c r="C105" t="s">
         <v>21</v>
       </c>
       <c r="D105" t="s">
-        <v>322</v>
+        <v>298</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>323</v>
+        <v>299</v>
       </c>
       <c r="B106" t="s">
-        <v>324</v>
+        <v>300</v>
       </c>
       <c r="C106" t="s">
         <v>77</v>
       </c>
       <c r="D106" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>326</v>
+        <v>302</v>
       </c>
       <c r="B107" t="s">
-        <v>327</v>
+        <v>303</v>
       </c>
       <c r="C107" t="s">
-        <v>189</v>
+        <v>96</v>
       </c>
       <c r="D107" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>329</v>
+        <v>305</v>
       </c>
       <c r="B108" t="s">
-        <v>330</v>
+        <v>306</v>
       </c>
       <c r="C108" t="s">
         <v>6</v>
       </c>
       <c r="D108" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>332</v>
+        <v>308</v>
       </c>
       <c r="B109" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="C109" t="s">
         <v>77</v>
       </c>
       <c r="D109" t="s">
-        <v>334</v>
+        <v>310</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>335</v>
+        <v>311</v>
       </c>
       <c r="B110" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="C110" t="s">
         <v>17</v>
       </c>
       <c r="D110" t="s">
-        <v>337</v>
+        <v>313</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
       <c r="B111" t="s">
-        <v>339</v>
+        <v>315</v>
       </c>
       <c r="C111" t="s">
         <v>77</v>
       </c>
       <c r="D111" t="s">
-        <v>340</v>
+        <v>316</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
       <c r="B112" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
       <c r="C112" t="s">
         <v>17</v>
       </c>
       <c r="D112" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>344</v>
+        <v>320</v>
       </c>
       <c r="B113" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="C113" t="s">
-        <v>189</v>
+        <v>96</v>
       </c>
       <c r="D113" t="s">
-        <v>346</v>
+        <v>322</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="B114" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="C114" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D114" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>350</v>
+        <v>326</v>
       </c>
       <c r="B115" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
       <c r="C115" t="s">
         <v>21</v>
       </c>
       <c r="D115" t="s">
-        <v>352</v>
+        <v>328</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>353</v>
+        <v>329</v>
       </c>
       <c r="B116" t="s">
-        <v>354</v>
+        <v>330</v>
       </c>
       <c r="C116" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D116" t="s">
-        <v>355</v>
+        <v>331</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>356</v>
+        <v>332</v>
       </c>
       <c r="B117" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
       <c r="C117" t="s">
         <v>6</v>
       </c>
       <c r="D117" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
       <c r="B118" t="s">
-        <v>360</v>
+        <v>336</v>
       </c>
       <c r="C118" t="s">
         <v>17</v>
       </c>
       <c r="D118" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>362</v>
+        <v>338</v>
       </c>
       <c r="B119" t="s">
-        <v>363</v>
+        <v>339</v>
       </c>
       <c r="C119" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D119" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>365</v>
+        <v>341</v>
       </c>
       <c r="B120" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="C120" t="s">
         <v>6</v>
       </c>
       <c r="D120" t="s">
-        <v>367</v>
+        <v>343</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>368</v>
+        <v>344</v>
       </c>
       <c r="B121" t="s">
-        <v>369</v>
+        <v>345</v>
       </c>
       <c r="C121" t="s">
         <v>10</v>
       </c>
       <c r="D121" t="s">
-        <v>370</v>
+        <v>346</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="B122" t="s">
-        <v>372</v>
+        <v>348</v>
       </c>
       <c r="C122" t="s">
         <v>6</v>
       </c>
       <c r="D122" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>374</v>
+        <v>350</v>
       </c>
       <c r="B123" t="s">
-        <v>375</v>
+        <v>351</v>
       </c>
       <c r="C123" t="s">
         <v>6</v>
       </c>
       <c r="D123" t="s">
-        <v>376</v>
+        <v>352</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>377</v>
+        <v>353</v>
       </c>
       <c r="B124" t="s">
-        <v>378</v>
+        <v>354</v>
       </c>
       <c r="C124" t="s">
         <v>6</v>
       </c>
       <c r="D124" t="s">
-        <v>379</v>
+        <v>355</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" t="s">
-        <v>380</v>
+        <v>356</v>
       </c>
       <c r="B125" t="s">
-        <v>381</v>
+        <v>357</v>
       </c>
       <c r="C125" t="s">
         <v>21</v>
       </c>
       <c r="D125" t="s">
-        <v>382</v>
+        <v>358</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="B126" t="s">
-        <v>384</v>
+        <v>360</v>
       </c>
       <c r="C126" t="s">
         <v>17</v>
       </c>
       <c r="D126" t="s">
-        <v>385</v>
+        <v>361</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" t="s">
-        <v>386</v>
+        <v>362</v>
       </c>
       <c r="B127" t="s">
-        <v>387</v>
+        <v>363</v>
       </c>
       <c r="C127" t="s">
         <v>17</v>
       </c>
       <c r="D127" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" t="s">
-        <v>389</v>
+        <v>365</v>
       </c>
       <c r="B128" t="s">
-        <v>390</v>
+        <v>366</v>
       </c>
       <c r="C128" t="s">
         <v>17</v>
       </c>
       <c r="D128" t="s">
-        <v>391</v>
+        <v>367</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" t="s">
-        <v>392</v>
+        <v>368</v>
       </c>
       <c r="B129" t="s">
-        <v>393</v>
+        <v>369</v>
       </c>
       <c r="C129" t="s">
         <v>34</v>
       </c>
       <c r="D129" t="s">
-        <v>394</v>
+        <v>370</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" t="s">
-        <v>395</v>
+        <v>371</v>
       </c>
       <c r="B130" t="s">
-        <v>396</v>
+        <v>372</v>
       </c>
       <c r="C130" t="s">
         <v>6</v>
       </c>
       <c r="D130" t="s">
-        <v>397</v>
+        <v>373</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
       <c r="B131" t="s">
-        <v>399</v>
+        <v>375</v>
       </c>
       <c r="C131" t="s">
         <v>77</v>
       </c>
       <c r="D131" t="s">
-        <v>400</v>
+        <v>376</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" t="s">
-        <v>401</v>
+        <v>377</v>
       </c>
       <c r="B132" t="s">
-        <v>402</v>
+        <v>378</v>
       </c>
       <c r="C132" t="s">
         <v>21</v>
       </c>
       <c r="D132" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" t="s">
-        <v>404</v>
+        <v>380</v>
       </c>
       <c r="B133" t="s">
-        <v>405</v>
+        <v>381</v>
       </c>
       <c r="C133" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D133" t="s">
-        <v>406</v>
+        <v>382</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" t="s">
-        <v>407</v>
+        <v>383</v>
       </c>
       <c r="B134" t="s">
-        <v>408</v>
+        <v>384</v>
       </c>
       <c r="C134" t="s">
         <v>10</v>
       </c>
       <c r="D134" t="s">
-        <v>409</v>
+        <v>385</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" t="s">
-        <v>410</v>
+        <v>386</v>
       </c>
       <c r="B135" t="s">
-        <v>411</v>
+        <v>387</v>
       </c>
       <c r="C135" t="s">
-        <v>412</v>
+        <v>388</v>
       </c>
       <c r="D135" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" t="s">
-        <v>414</v>
+        <v>390</v>
       </c>
       <c r="B136" t="s">
-        <v>415</v>
+        <v>391</v>
       </c>
       <c r="C136" t="s">
         <v>6</v>
       </c>
       <c r="D136" t="s">
-        <v>416</v>
+        <v>392</v>
       </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" t="s">
-        <v>417</v>
+        <v>393</v>
       </c>
       <c r="B137" t="s">
-        <v>418</v>
+        <v>394</v>
       </c>
       <c r="C137" t="s">
         <v>77</v>
       </c>
       <c r="D137" t="s">
-        <v>419</v>
+        <v>395</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" t="s">
-        <v>420</v>
+        <v>396</v>
       </c>
       <c r="B138" t="s">
-        <v>421</v>
+        <v>397</v>
       </c>
       <c r="C138" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D138" t="s">
-        <v>422</v>
+        <v>398</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" t="s">
-        <v>423</v>
+        <v>399</v>
       </c>
       <c r="B139" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
       <c r="C139" t="s">
         <v>17</v>
       </c>
       <c r="D139" t="s">
-        <v>425</v>
+        <v>401</v>
       </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" t="s">
-        <v>426</v>
+        <v>402</v>
       </c>
       <c r="B140" t="s">
-        <v>427</v>
+        <v>403</v>
       </c>
       <c r="C140" t="s">
         <v>77</v>
       </c>
       <c r="D140" t="s">
-        <v>428</v>
+        <v>404</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" t="s">
-        <v>429</v>
+        <v>405</v>
       </c>
       <c r="B141" t="s">
-        <v>430</v>
+        <v>406</v>
       </c>
       <c r="C141" t="s">
         <v>34</v>
       </c>
       <c r="D141" t="s">
-        <v>431</v>
+        <v>407</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" t="s">
-        <v>432</v>
+        <v>408</v>
       </c>
       <c r="B142" t="s">
-        <v>433</v>
+        <v>409</v>
       </c>
       <c r="C142" t="s">
         <v>77</v>
       </c>
       <c r="D142" t="s">
-        <v>434</v>
+        <v>410</v>
       </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" t="s">
-        <v>435</v>
+        <v>411</v>
       </c>
       <c r="B143" t="s">
-        <v>436</v>
+        <v>412</v>
       </c>
       <c r="C143" t="s">
         <v>6</v>
       </c>
       <c r="D143" t="s">
-        <v>437</v>
+        <v>413</v>
       </c>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" t="s">
-        <v>438</v>
+        <v>414</v>
       </c>
       <c r="B144" t="s">
-        <v>439</v>
+        <v>415</v>
       </c>
       <c r="C144" t="s">
         <v>6</v>
       </c>
       <c r="D144" t="s">
-        <v>440</v>
+        <v>416</v>
       </c>
     </row>
     <row r="145" spans="1:4">
       <c r="A145" t="s">
-        <v>441</v>
+        <v>417</v>
       </c>
       <c r="B145" t="s">
-        <v>442</v>
+        <v>418</v>
       </c>
       <c r="C145" t="s">
         <v>17</v>
       </c>
       <c r="D145" t="s">
-        <v>443</v>
+        <v>419</v>
       </c>
     </row>
     <row r="146" spans="1:4">
       <c r="A146" t="s">
-        <v>444</v>
+        <v>420</v>
       </c>
       <c r="B146" t="s">
-        <v>445</v>
+        <v>421</v>
       </c>
       <c r="C146" t="s">
         <v>6</v>
       </c>
       <c r="D146" t="s">
-        <v>446</v>
+        <v>422</v>
       </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" t="s">
-        <v>447</v>
+        <v>423</v>
       </c>
       <c r="B147" t="s">
-        <v>448</v>
+        <v>424</v>
       </c>
       <c r="C147" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D147" t="s">
-        <v>449</v>
+        <v>425</v>
       </c>
     </row>
     <row r="148" spans="1:4">
       <c r="A148" t="s">
-        <v>450</v>
+        <v>426</v>
       </c>
       <c r="B148" t="s">
-        <v>451</v>
+        <v>427</v>
       </c>
       <c r="C148" t="s">
         <v>17</v>
       </c>
       <c r="D148" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
     </row>
     <row r="149" spans="1:4">
       <c r="A149" t="s">
-        <v>453</v>
+        <v>429</v>
       </c>
       <c r="B149" t="s">
-        <v>454</v>
+        <v>430</v>
       </c>
       <c r="C149" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D149" t="s">
-        <v>455</v>
+        <v>431</v>
       </c>
     </row>
     <row r="150" spans="1:4">
       <c r="A150" t="s">
-        <v>456</v>
+        <v>432</v>
       </c>
       <c r="B150" t="s">
-        <v>457</v>
+        <v>433</v>
       </c>
       <c r="C150" t="s">
         <v>17</v>
       </c>
       <c r="D150" t="s">
-        <v>458</v>
+        <v>434</v>
       </c>
     </row>
     <row r="151" spans="1:4">
       <c r="A151" t="s">
-        <v>459</v>
+        <v>435</v>
       </c>
       <c r="B151" t="s">
-        <v>460</v>
+        <v>436</v>
       </c>
       <c r="C151" t="s">
         <v>6</v>
       </c>
       <c r="D151" t="s">
-        <v>461</v>
+        <v>437</v>
       </c>
     </row>
     <row r="152" spans="1:4">
       <c r="A152" t="s">
-        <v>462</v>
+        <v>438</v>
       </c>
       <c r="B152" t="s">
-        <v>463</v>
+        <v>439</v>
       </c>
       <c r="C152" t="s">
         <v>10</v>
       </c>
       <c r="D152" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="153" spans="1:4">
       <c r="A153" t="s">
-        <v>465</v>
+        <v>441</v>
       </c>
       <c r="B153" t="s">
-        <v>466</v>
+        <v>442</v>
       </c>
       <c r="C153" t="s">
-        <v>189</v>
+        <v>96</v>
       </c>
       <c r="D153" t="s">
-        <v>467</v>
+        <v>443</v>
       </c>
     </row>
     <row r="154" spans="1:4">
       <c r="A154" t="s">
-        <v>468</v>
+        <v>444</v>
       </c>
       <c r="B154" t="s">
-        <v>469</v>
+        <v>445</v>
       </c>
       <c r="C154" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D154" t="s">
-        <v>470</v>
+        <v>446</v>
       </c>
     </row>
     <row r="155" spans="1:4">
       <c r="A155" t="s">
-        <v>471</v>
+        <v>447</v>
       </c>
       <c r="B155" t="s">
-        <v>472</v>
+        <v>448</v>
       </c>
       <c r="C155" t="s">
         <v>17</v>
       </c>
       <c r="D155" t="s">
-        <v>473</v>
+        <v>449</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" t="s">
-        <v>474</v>
+        <v>450</v>
       </c>
       <c r="B156" t="s">
-        <v>475</v>
+        <v>451</v>
       </c>
       <c r="C156" t="s">
         <v>6</v>
       </c>
       <c r="D156" t="s">
-        <v>476</v>
+        <v>452</v>
       </c>
     </row>
     <row r="157" spans="1:4">
       <c r="A157" t="s">
-        <v>477</v>
+        <v>453</v>
       </c>
       <c r="B157" t="s">
-        <v>478</v>
+        <v>454</v>
       </c>
       <c r="C157" t="s">
         <v>6</v>
       </c>
       <c r="D157" t="s">
-        <v>479</v>
+        <v>455</v>
       </c>
     </row>
     <row r="158" spans="1:4">
       <c r="A158" t="s">
-        <v>480</v>
+        <v>456</v>
       </c>
       <c r="B158" t="s">
-        <v>481</v>
+        <v>457</v>
       </c>
       <c r="C158" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D158" t="s">
-        <v>482</v>
+        <v>458</v>
       </c>
     </row>
     <row r="159" spans="1:4">
       <c r="A159" t="s">
-        <v>483</v>
+        <v>459</v>
       </c>
       <c r="B159" t="s">
-        <v>484</v>
+        <v>460</v>
       </c>
       <c r="C159" t="s">
         <v>77</v>
       </c>
       <c r="D159" t="s">
-        <v>485</v>
+        <v>461</v>
       </c>
     </row>
     <row r="160" spans="1:4">
       <c r="A160" t="s">
-        <v>486</v>
+        <v>462</v>
       </c>
       <c r="B160" t="s">
-        <v>487</v>
+        <v>463</v>
       </c>
       <c r="C160" t="s">
-        <v>412</v>
+        <v>388</v>
       </c>
       <c r="D160" t="s">
-        <v>488</v>
+        <v>464</v>
       </c>
     </row>
     <row r="161" spans="1:4">
       <c r="A161" t="s">
-        <v>489</v>
+        <v>465</v>
       </c>
       <c r="B161" t="s">
-        <v>490</v>
+        <v>466</v>
       </c>
       <c r="C161" t="s">
         <v>10</v>
       </c>
       <c r="D161" t="s">
-        <v>491</v>
+        <v>467</v>
       </c>
     </row>
     <row r="162" spans="1:4">
       <c r="A162" t="s">
-        <v>492</v>
+        <v>468</v>
       </c>
       <c r="B162" t="s">
-        <v>493</v>
+        <v>469</v>
       </c>
       <c r="C162" t="s">
         <v>6</v>
       </c>
       <c r="D162" t="s">
-        <v>494</v>
+        <v>470</v>
       </c>
     </row>
     <row r="163" spans="1:4">
       <c r="A163" t="s">
-        <v>495</v>
+        <v>471</v>
       </c>
       <c r="B163" t="s">
-        <v>496</v>
+        <v>472</v>
       </c>
       <c r="C163" t="s">
         <v>17</v>
       </c>
       <c r="D163" t="s">
-        <v>497</v>
+        <v>473</v>
       </c>
     </row>
     <row r="164" spans="1:4">
       <c r="A164" t="s">
-        <v>498</v>
+        <v>474</v>
       </c>
       <c r="B164" t="s">
-        <v>499</v>
+        <v>475</v>
       </c>
       <c r="C164" t="s">
         <v>77</v>
       </c>
       <c r="D164" t="s">
-        <v>500</v>
+        <v>476</v>
       </c>
     </row>
     <row r="165" spans="1:4">
       <c r="A165" t="s">
-        <v>501</v>
+        <v>477</v>
       </c>
       <c r="B165" t="s">
-        <v>502</v>
+        <v>478</v>
       </c>
       <c r="C165" t="s">
         <v>17</v>
       </c>
       <c r="D165" t="s">
-        <v>503</v>
+        <v>479</v>
       </c>
     </row>
     <row r="166" spans="1:4">
       <c r="A166" t="s">
-        <v>504</v>
+        <v>480</v>
       </c>
       <c r="B166" t="s">
-        <v>505</v>
+        <v>481</v>
       </c>
       <c r="C166" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D166" t="s">
-        <v>506</v>
+        <v>482</v>
       </c>
     </row>
     <row r="167" spans="1:4">
       <c r="A167" t="s">
-        <v>507</v>
+        <v>483</v>
       </c>
       <c r="B167" t="s">
-        <v>508</v>
+        <v>484</v>
       </c>
       <c r="C167" t="s">
         <v>10</v>
       </c>
       <c r="D167" t="s">
-        <v>509</v>
+        <v>485</v>
       </c>
     </row>
     <row r="168" spans="1:4">
       <c r="A168" t="s">
-        <v>510</v>
+        <v>486</v>
       </c>
       <c r="B168" t="s">
-        <v>511</v>
+        <v>487</v>
       </c>
       <c r="C168" t="s">
         <v>21</v>
       </c>
       <c r="D168" t="s">
-        <v>512</v>
+        <v>488</v>
       </c>
     </row>
     <row r="169" spans="1:4">
       <c r="A169" t="s">
-        <v>513</v>
+        <v>489</v>
       </c>
       <c r="B169" t="s">
-        <v>514</v>
+        <v>490</v>
       </c>
       <c r="C169" t="s">
         <v>17</v>
       </c>
       <c r="D169" t="s">
-        <v>515</v>
+        <v>491</v>
       </c>
     </row>
     <row r="170" spans="1:4">
       <c r="A170" t="s">
-        <v>516</v>
+        <v>492</v>
       </c>
       <c r="B170" t="s">
-        <v>517</v>
+        <v>493</v>
       </c>
       <c r="C170" t="s">
         <v>17</v>
       </c>
       <c r="D170" t="s">
-        <v>518</v>
+        <v>494</v>
       </c>
     </row>
     <row r="171" spans="1:4">
       <c r="A171" t="s">
-        <v>519</v>
+        <v>495</v>
       </c>
       <c r="B171" t="s">
-        <v>445</v>
+        <v>421</v>
       </c>
       <c r="C171" t="s">
         <v>6</v>
       </c>
       <c r="D171" t="s">
-        <v>520</v>
+        <v>496</v>
       </c>
     </row>
     <row r="172" spans="1:4">
       <c r="A172" t="s">
-        <v>521</v>
+        <v>497</v>
       </c>
       <c r="B172" t="s">
-        <v>522</v>
+        <v>498</v>
       </c>
       <c r="C172" t="s">
         <v>34</v>
       </c>
       <c r="D172" t="s">
-        <v>523</v>
+        <v>499</v>
       </c>
     </row>
     <row r="173" spans="1:4">
       <c r="A173" t="s">
-        <v>524</v>
+        <v>500</v>
       </c>
       <c r="B173" t="s">
-        <v>525</v>
+        <v>501</v>
       </c>
       <c r="C173" t="s">
         <v>10</v>
       </c>
       <c r="D173" t="s">
-        <v>526</v>
+        <v>502</v>
       </c>
     </row>
     <row r="174" spans="1:4">
       <c r="A174" t="s">
-        <v>527</v>
+        <v>503</v>
       </c>
       <c r="B174" t="s">
-        <v>528</v>
+        <v>504</v>
       </c>
       <c r="C174" t="s">
         <v>10</v>
       </c>
       <c r="D174" t="s">
-        <v>529</v>
+        <v>505</v>
       </c>
     </row>
     <row r="175" spans="1:4">
       <c r="A175" t="s">
-        <v>530</v>
+        <v>506</v>
       </c>
       <c r="B175" t="s">
-        <v>531</v>
+        <v>507</v>
       </c>
       <c r="C175" t="s">
         <v>10</v>
       </c>
       <c r="D175" t="s">
-        <v>532</v>
+        <v>508</v>
       </c>
     </row>
     <row r="176" spans="1:4">
       <c r="A176" t="s">
-        <v>533</v>
+        <v>509</v>
       </c>
       <c r="B176" t="s">
-        <v>534</v>
+        <v>510</v>
       </c>
       <c r="C176" t="s">
         <v>17</v>
       </c>
       <c r="D176" t="s">
-        <v>535</v>
+        <v>511</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177" t="s">
-        <v>536</v>
+        <v>512</v>
       </c>
       <c r="B177" t="s">
-        <v>537</v>
+        <v>513</v>
       </c>
       <c r="C177" t="s">
         <v>17</v>
       </c>
       <c r="D177" t="s">
-        <v>538</v>
+        <v>514</v>
       </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178" t="s">
-        <v>539</v>
+        <v>515</v>
       </c>
       <c r="B178" t="s">
-        <v>540</v>
+        <v>516</v>
       </c>
       <c r="C178" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D178" t="s">
-        <v>541</v>
+        <v>517</v>
       </c>
     </row>
     <row r="179" spans="1:4">
       <c r="A179" t="s">
-        <v>542</v>
+        <v>518</v>
       </c>
       <c r="B179" t="s">
-        <v>543</v>
+        <v>519</v>
       </c>
       <c r="C179" t="s">
-        <v>412</v>
+        <v>388</v>
       </c>
       <c r="D179" t="s">
-        <v>544</v>
+        <v>520</v>
       </c>
     </row>
     <row r="180" spans="1:4">
       <c r="A180" t="s">
-        <v>545</v>
+        <v>521</v>
       </c>
       <c r="B180" t="s">
-        <v>546</v>
+        <v>522</v>
       </c>
       <c r="C180" t="s">
         <v>17</v>
       </c>
       <c r="D180" t="s">
-        <v>547</v>
+        <v>523</v>
       </c>
     </row>
     <row r="181" spans="1:4">
       <c r="A181" t="s">
-        <v>548</v>
+        <v>524</v>
       </c>
       <c r="B181" t="s">
-        <v>549</v>
+        <v>525</v>
       </c>
       <c r="C181" t="s">
         <v>6</v>
       </c>
       <c r="D181" t="s">
-        <v>550</v>
+        <v>526</v>
       </c>
     </row>
     <row r="182" spans="1:4">
       <c r="A182" t="s">
-        <v>551</v>
+        <v>527</v>
       </c>
       <c r="B182" t="s">
-        <v>552</v>
+        <v>528</v>
       </c>
       <c r="C182" t="s">
-        <v>412</v>
+        <v>388</v>
       </c>
       <c r="D182" t="s">
-        <v>553</v>
+        <v>529</v>
       </c>
     </row>
     <row r="183" spans="1:4">
       <c r="A183" t="s">
-        <v>554</v>
+        <v>530</v>
       </c>
       <c r="B183" t="s">
-        <v>555</v>
+        <v>531</v>
       </c>
       <c r="C183" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D183" t="s">
-        <v>556</v>
+        <v>532</v>
       </c>
     </row>
     <row r="184" spans="1:4">
       <c r="A184" t="s">
-        <v>557</v>
+        <v>533</v>
       </c>
       <c r="B184" t="s">
-        <v>558</v>
+        <v>534</v>
       </c>
       <c r="C184" t="s">
         <v>21</v>
       </c>
       <c r="D184" t="s">
-        <v>559</v>
+        <v>535</v>
       </c>
     </row>
     <row r="185" spans="1:4">
       <c r="A185" t="s">
-        <v>560</v>
+        <v>536</v>
       </c>
       <c r="B185" t="s">
-        <v>561</v>
+        <v>537</v>
       </c>
       <c r="C185" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D185" t="s">
-        <v>562</v>
+        <v>538</v>
       </c>
     </row>
     <row r="186" spans="1:4">
       <c r="A186" t="s">
-        <v>563</v>
+        <v>539</v>
       </c>
       <c r="B186" t="s">
-        <v>564</v>
+        <v>540</v>
       </c>
       <c r="C186" t="s">
         <v>10</v>
       </c>
       <c r="D186" t="s">
-        <v>565</v>
+        <v>541</v>
       </c>
     </row>
     <row r="187" spans="1:4">
       <c r="A187" t="s">
-        <v>566</v>
+        <v>542</v>
       </c>
       <c r="B187" t="s">
-        <v>567</v>
+        <v>543</v>
       </c>
       <c r="C187" t="s">
         <v>17</v>
       </c>
       <c r="D187" t="s">
-        <v>568</v>
+        <v>544</v>
       </c>
     </row>
     <row r="188" spans="1:4">
       <c r="A188" t="s">
-        <v>569</v>
+        <v>545</v>
       </c>
       <c r="B188" t="s">
-        <v>570</v>
+        <v>546</v>
       </c>
       <c r="C188" t="s">
         <v>77</v>
       </c>
       <c r="D188" t="s">
-        <v>571</v>
+        <v>547</v>
       </c>
     </row>
     <row r="189" spans="1:4">
       <c r="A189" t="s">
-        <v>572</v>
+        <v>548</v>
       </c>
       <c r="B189" t="s">
-        <v>573</v>
+        <v>549</v>
       </c>
       <c r="C189" t="s">
         <v>17</v>
       </c>
       <c r="D189" t="s">
-        <v>574</v>
+        <v>550</v>
       </c>
     </row>
     <row r="190" spans="1:4">
       <c r="A190" t="s">
-        <v>575</v>
+        <v>551</v>
       </c>
       <c r="B190" t="s">
-        <v>576</v>
+        <v>552</v>
       </c>
       <c r="C190" t="s">
         <v>21</v>
       </c>
       <c r="D190" t="s">
-        <v>577</v>
+        <v>553</v>
       </c>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" t="s">
-        <v>578</v>
+        <v>554</v>
       </c>
       <c r="B191" t="s">
-        <v>579</v>
+        <v>555</v>
       </c>
       <c r="C191" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D191" t="s">
-        <v>580</v>
+        <v>556</v>
       </c>
     </row>
     <row r="192" spans="1:4">
       <c r="A192" t="s">
-        <v>581</v>
+        <v>557</v>
       </c>
       <c r="B192" t="s">
-        <v>582</v>
+        <v>558</v>
       </c>
       <c r="C192" t="s">
         <v>10</v>
       </c>
       <c r="D192" t="s">
-        <v>583</v>
+        <v>559</v>
       </c>
     </row>
     <row r="193" spans="1:4">
       <c r="A193" t="s">
-        <v>584</v>
+        <v>560</v>
       </c>
       <c r="B193" t="s">
-        <v>585</v>
+        <v>561</v>
       </c>
       <c r="C193" t="s">
         <v>34</v>
       </c>
       <c r="D193" t="s">
-        <v>586</v>
+        <v>562</v>
       </c>
     </row>
     <row r="194" spans="1:4">
       <c r="A194" t="s">
-        <v>587</v>
+        <v>563</v>
       </c>
       <c r="B194" t="s">
-        <v>588</v>
+        <v>564</v>
       </c>
       <c r="C194" t="s">
         <v>17</v>
       </c>
       <c r="D194" t="s">
-        <v>589</v>
+        <v>565</v>
       </c>
     </row>
     <row r="195" spans="1:4">
       <c r="A195" t="s">
-        <v>590</v>
+        <v>566</v>
       </c>
       <c r="B195" t="s">
-        <v>591</v>
+        <v>567</v>
       </c>
       <c r="C195" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D195" t="s">
-        <v>592</v>
+        <v>568</v>
       </c>
     </row>
     <row r="196" spans="1:4">
       <c r="A196" t="s">
-        <v>593</v>
+        <v>569</v>
       </c>
       <c r="B196" t="s">
-        <v>594</v>
+        <v>570</v>
       </c>
       <c r="C196" t="s">
         <v>6</v>
       </c>
       <c r="D196" t="s">
-        <v>595</v>
+        <v>571</v>
       </c>
     </row>
     <row r="197" spans="1:4">
       <c r="A197" t="s">
-        <v>596</v>
+        <v>572</v>
       </c>
       <c r="B197" t="s">
-        <v>597</v>
+        <v>573</v>
       </c>
       <c r="C197" t="s">
         <v>34</v>
       </c>
       <c r="D197" t="s">
-        <v>598</v>
+        <v>574</v>
       </c>
     </row>
     <row r="198" spans="1:4">
       <c r="A198" t="s">
-        <v>599</v>
+        <v>575</v>
       </c>
       <c r="B198" t="s">
-        <v>600</v>
+        <v>576</v>
       </c>
       <c r="C198" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D198" t="s">
-        <v>601</v>
+        <v>577</v>
       </c>
     </row>
     <row r="199" spans="1:4">
       <c r="A199" t="s">
-        <v>602</v>
+        <v>578</v>
       </c>
       <c r="B199" t="s">
-        <v>603</v>
+        <v>579</v>
       </c>
       <c r="C199" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D199" t="s">
-        <v>604</v>
+        <v>580</v>
       </c>
     </row>
     <row r="200" spans="1:4">
       <c r="A200" t="s">
-        <v>605</v>
+        <v>581</v>
       </c>
       <c r="B200" t="s">
-        <v>606</v>
+        <v>582</v>
       </c>
       <c r="C200" t="s">
         <v>34</v>
       </c>
       <c r="D200" t="s">
-        <v>607</v>
+        <v>583</v>
       </c>
     </row>
     <row r="201" spans="1:4">
       <c r="A201" t="s">
-        <v>608</v>
+        <v>584</v>
       </c>
       <c r="B201" t="s">
-        <v>609</v>
+        <v>585</v>
       </c>
       <c r="C201" t="s">
         <v>77</v>
       </c>
       <c r="D201" t="s">
-        <v>610</v>
+        <v>586</v>
       </c>
     </row>
     <row r="202" spans="1:4">
       <c r="A202" t="s">
-        <v>611</v>
+        <v>587</v>
       </c>
       <c r="B202" t="s">
-        <v>612</v>
+        <v>588</v>
       </c>
       <c r="C202" t="s">
         <v>21</v>
       </c>
       <c r="D202" t="s">
-        <v>613</v>
+        <v>589</v>
       </c>
     </row>
     <row r="203" spans="1:4">
       <c r="A203" t="s">
-        <v>614</v>
+        <v>590</v>
       </c>
       <c r="B203" t="s">
-        <v>615</v>
+        <v>591</v>
       </c>
       <c r="C203" t="s">
-        <v>189</v>
+        <v>96</v>
       </c>
       <c r="D203" t="s">
-        <v>616</v>
+        <v>592</v>
       </c>
     </row>
     <row r="204" spans="1:4">
       <c r="A204" t="s">
-        <v>617</v>
+        <v>593</v>
       </c>
       <c r="B204" t="s">
-        <v>618</v>
+        <v>594</v>
       </c>
       <c r="C204" t="s">
         <v>34</v>
       </c>
       <c r="D204" t="s">
-        <v>619</v>
+        <v>595</v>
       </c>
     </row>
     <row r="205" spans="1:4">
       <c r="A205" t="s">
-        <v>620</v>
+        <v>596</v>
       </c>
       <c r="B205" t="s">
-        <v>621</v>
+        <v>597</v>
       </c>
       <c r="C205" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D205" t="s">
-        <v>622</v>
+        <v>598</v>
       </c>
     </row>
     <row r="206" spans="1:4">
       <c r="A206" t="s">
-        <v>623</v>
+        <v>599</v>
       </c>
       <c r="B206" t="s">
-        <v>624</v>
+        <v>600</v>
       </c>
       <c r="C206" t="s">
-        <v>189</v>
+        <v>96</v>
       </c>
       <c r="D206" t="s">
-        <v>625</v>
+        <v>601</v>
       </c>
     </row>
     <row r="207" spans="1:4">
       <c r="A207" t="s">
-        <v>626</v>
+        <v>602</v>
       </c>
       <c r="B207" t="s">
-        <v>627</v>
+        <v>603</v>
       </c>
       <c r="C207" t="s">
         <v>34</v>
       </c>
       <c r="D207" t="s">
-        <v>628</v>
+        <v>604</v>
       </c>
     </row>
   </sheetData>

</xml_diff>